<commit_message>
add log4j2 && add more test case for create account, course
</commit_message>
<xml_diff>
--- a/document/DD_EditCourse.xlsx
+++ b/document/DD_EditCourse.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="1110" windowWidth="9210" windowHeight="6465" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="19110" windowHeight="7575" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="1" r:id="rId1"/>
@@ -944,6 +944,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="ＭＳ ゴシック"/>
+        <charset val="128"/>
+      </rPr>
       <t>format(yyyy-MM-</t>
     </r>
     <r>
@@ -965,6 +970,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="ＭＳ ゴシック"/>
+        <charset val="128"/>
+      </rPr>
       <t>Ngày k</t>
     </r>
     <r>
@@ -1011,6 +1021,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="ＭＳ ゴシック"/>
+        <charset val="128"/>
+      </rPr>
       <t>H</t>
     </r>
     <r>
@@ -1035,6 +1050,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="ＭＳ ゴシック"/>
+        <charset val="128"/>
+      </rPr>
       <t>Khuy</t>
     </r>
     <r>
@@ -1103,6 +1123,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="163"/>
+      </rPr>
       <t>決済</t>
     </r>
     <r>
@@ -1345,14 +1370,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="0.0_ "/>
-    <numFmt numFmtId="178" formatCode="yy/mm/dd"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="yy/mm/dd"/>
   </numFmts>
   <fonts count="69">
     <font>
@@ -1615,36 +1640,28 @@
       <charset val="128"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1659,17 +1676,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1696,14 +1734,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1711,8 +1741,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1726,40 +1781,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1817,19 +1842,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1841,25 +1866,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1877,13 +1902,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1895,25 +1980,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1925,49 +1998,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1979,25 +2022,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2184,26 +2209,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2264,6 +2274,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -2272,152 +2306,143 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="55" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="17" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="58" fillId="12" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="46" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="50" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="47" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="53" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="16" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="57" fillId="16" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="56" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="47" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="47" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="46" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="50" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="46" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="46" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="48" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="47" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="61" fillId="21" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="46" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="47" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2602,7 +2627,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="12" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="12" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="35" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2800,10 +2825,10 @@
     <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="35" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="18" fillId="0" borderId="12" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="18" fillId="0" borderId="12" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="18" fillId="0" borderId="6" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="18" fillId="0" borderId="6" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="13" xfId="35" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2994,7 +3019,7 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="6" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="0" borderId="6" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3021,7 +3046,7 @@
     <xf numFmtId="177" fontId="18" fillId="0" borderId="6" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="18" fillId="0" borderId="6" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="6" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="58" fontId="18" fillId="0" borderId="6" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4277,12 +4302,12 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="" altLang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
+            <a:rPr lang="en-US" altLang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
               <a:latin typeface="Times New Roman" pitchFamily="12"/>
             </a:rPr>
             <a:t>course</a:t>
           </a:r>
-          <a:endParaRPr lang="" altLang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
+          <a:endParaRPr lang="en-US" altLang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
             <a:latin typeface="Times New Roman" pitchFamily="12"/>
           </a:endParaRPr>
         </a:p>
@@ -5313,7 +5338,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -5480,8 +5505,8 @@
   </sheetPr>
   <dimension ref="B1:BK67"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="AB38" sqref="AB38:AF39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -9776,7 +9801,7 @@
     <mergeCell ref="B1:L2"/>
   </mergeCells>
   <pageMargins left="0.39375" right="0.39375" top="0.590277777777778" bottom="0.590972222222222" header="0.511805555555555" footer="0.315277777777778"/>
-  <pageSetup paperSize="9" scale="36" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="34" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;"Arial,Regular"&amp;P</oddFooter>
   </headerFooter>
@@ -9791,8 +9816,8 @@
   </sheetPr>
   <dimension ref="A1:CR64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4:BM4"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AK9" sqref="AK9:AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -15231,8 +15256,8 @@
   </sheetPr>
   <dimension ref="B1:BI65"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:AG46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -19558,7 +19583,7 @@
     <mergeCell ref="AT6:BF7"/>
   </mergeCells>
   <pageMargins left="0.39375" right="0.39375" top="0.590277777777778" bottom="0.590972222222222" header="0.511805555555555" footer="0.315277777777778"/>
-  <pageSetup paperSize="9" scale="39" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="38" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;"Arial,Regular"&amp;P</oddFooter>
   </headerFooter>

</xml_diff>